<commit_message>
implemented data generation script
</commit_message>
<xml_diff>
--- a/Runtimes.xlsx
+++ b/Runtimes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E55B241-0592-4B22-A141-4EB2F2ECD1D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C3BC6-B332-4606-B39B-37C835D5B243}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Runtimes (30 rounds)</t>
   </si>
@@ -49,19 +49,28 @@
     <t>------------</t>
   </si>
   <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>v^2</t>
-  </si>
-  <si>
     <t>Shortest Path</t>
   </si>
   <si>
     <t>Filter = Selected for each field</t>
   </si>
   <si>
-    <t>v + e</t>
+    <t>Big O notation</t>
+  </si>
+  <si>
+    <t>Estimated Runtimes (for Actual Data)</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>O(v)</t>
+  </si>
+  <si>
+    <t>O(v^2)</t>
+  </si>
+  <si>
+    <t>O(v + e)</t>
   </si>
 </sst>
 </file>
@@ -403,7 +412,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,10 +422,12 @@
     <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -425,11 +436,17 @@
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -443,8 +460,11 @@
       <c r="E2" s="1">
         <v>7</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6.8496465682983398E-3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -462,7 +482,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1">
         <f>C3/5*50</f>
@@ -484,7 +504,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1">
         <f>C4/5*(50^2)</f>
@@ -494,7 +514,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>4.7209421793619703E-3</v>
@@ -506,7 +526,11 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="G5" s="1">
+        <f>C5/5*(50^2)</f>
+        <v>2.3604710896809853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Bugs and made the plotting work
</commit_message>
<xml_diff>
--- a/Runtimes.xlsx
+++ b/Runtimes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C3BC6-B332-4606-B39B-37C835D5B243}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E593C6E2-E9AF-4ECF-8605-21177CCA2CB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -452,7 +452,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>6.8496465682983398E-3</v>
+        <v>4.9205938975016199E-3</v>
       </c>
       <c r="D2" s="1">
         <v>7</v>
@@ -473,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>7.0144812266031897E-3</v>
+        <v>5.0545771916707298E-3</v>
       </c>
       <c r="D3" s="1">
         <v>17</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="G3" s="1">
         <f>C3/5*50</f>
-        <v>7.0144812266031906E-2</v>
+        <v>5.0545771916707297E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>7.1807543436686197E-3</v>
+        <v>5.2857319513956698E-3</v>
       </c>
       <c r="D4" s="1">
         <v>21</v>
@@ -508,7 +508,7 @@
       </c>
       <c r="G4" s="1">
         <f>C4/5*(50^2)</f>
-        <v>3.59037717183431</v>
+        <v>2.642865975697835</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>